<commit_message>
Add notes on search
</commit_message>
<xml_diff>
--- a/gradu/material_search.xlsx
+++ b/gradu/material_search.xlsx
@@ -20,9 +20,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Material search results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepted</t>
   </si>
 </sst>
 </file>
@@ -32,11 +50,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -58,9 +77,17 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,8 +96,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF158466"/>
+        <fgColor rgb="FF168253"/>
         <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFDDE8CB"/>
       </patternFill>
     </fill>
   </fills>
@@ -83,7 +122,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -107,14 +146,19 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -122,15 +166,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading 1" xfId="20"/>
+    <cellStyle name="Heading 1 1" xfId="20"/>
+    <cellStyle name="Heading 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -147,8 +200,8 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF158466"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF168253"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -168,7 +221,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFDDE8CB"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -200,20 +253,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="J1:L1"/>
+  <dimension ref="J1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="65.91"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>